<commit_message>
Corrected routing due to EC remarks, no placement (or other) change
</commit_message>
<xml_diff>
--- a/Project Outputs for VHF_AMP/BOM/Bill of Materials-VHF_AMP(std).xlsx
+++ b/Project Outputs for VHF_AMP/BOM/Bill of Materials-VHF_AMP(std).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Magazyn_TachBook\My Work\INNE\VHF_Amp\Project Outputs for VHF_AMP\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88DB2308-A29D-49E1-B9AB-63E84F1AB4A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3CFF2554-6C04-4A8B-B31C-7A0F7E596F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19515" yWindow="1035" windowWidth="7500" windowHeight="6000" xr2:uid="{D759F41C-AE8E-4BBC-B61B-61E50EBD7513}"/>
+    <workbookView xWindow="19515" yWindow="1035" windowWidth="7500" windowHeight="6000" xr2:uid="{84377CA4-5872-4623-A0D9-CE123B06C859}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-VHF_AMP(std)" sheetId="1" r:id="rId1"/>
@@ -2676,7 +2676,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F9E1F8A-8A36-416A-B100-853BD5BB4B14}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53AD2067-7A6B-462E-BDB1-5E6B28FF497D}">
   <dimension ref="A1:L150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>